<commit_message>
update after taking the second field exam
</commit_message>
<xml_diff>
--- a/meredith/field exam papers and topics.xlsx
+++ b/meredith/field exam papers and topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\github\are261\meredith\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B11F6A-D773-48B4-BA57-BCD9D8BA8477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191AC372-40E5-492B-AC04-D5E3516E4F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40EFB020-B7E7-4026-AAC0-97F111614357}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Calendar" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Readings!$A$1:$H$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Readings!$A$1:$I$126</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="298">
   <si>
     <t>Professor</t>
   </si>
@@ -1335,11 +1335,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC9AABE-D912-4539-92BB-AE21E65F9BAF}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H130" sqref="H130"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I118" sqref="I118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,14 +1349,14 @@
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" customWidth="1"/>
-    <col min="8" max="8" width="60.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+    <col min="9" max="9" width="60.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1375,14 +1375,15 @@
       <c r="F1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -1401,14 +1402,14 @@
       <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -1424,14 +1425,14 @@
       <c r="F3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1447,14 +1448,14 @@
       <c r="F4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1473,14 +1474,14 @@
       <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -1499,14 +1500,14 @@
       <c r="F6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1522,14 +1523,14 @@
       <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -1548,14 +1549,14 @@
       <c r="F8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -1574,14 +1575,14 @@
       <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1600,14 +1601,14 @@
       <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -1623,14 +1624,14 @@
       <c r="F11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -1649,14 +1650,14 @@
       <c r="F12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>282</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -1675,14 +1676,14 @@
       <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -1698,14 +1699,14 @@
       <c r="F14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -1721,14 +1722,14 @@
       <c r="F15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1744,14 +1745,14 @@
       <c r="F16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -1770,14 +1771,14 @@
       <c r="F17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -1793,14 +1794,14 @@
       <c r="F18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -1819,14 +1820,14 @@
       <c r="F19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -1845,14 +1846,14 @@
       <c r="F20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1868,14 +1869,14 @@
       <c r="F21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -1894,14 +1895,14 @@
       <c r="F22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1920,14 +1921,14 @@
       <c r="F23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -1946,14 +1947,14 @@
       <c r="F24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -1969,14 +1970,17 @@
       <c r="F25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -1992,14 +1996,17 @@
       <c r="F26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="2">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
         <v>88</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -2015,14 +2022,17 @@
       <c r="F27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="2">
+        <v>3</v>
+      </c>
+      <c r="H27" t="s">
         <v>100</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -2041,14 +2051,17 @@
       <c r="F28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2">
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -2064,14 +2077,17 @@
       <c r="F29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
         <v>92</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>124</v>
       </c>
@@ -2090,14 +2106,17 @@
       <c r="F30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
         <v>65</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -2113,14 +2132,17 @@
       <c r="F31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="2">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
         <v>110</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -2139,14 +2161,17 @@
       <c r="F32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="2">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -2165,14 +2190,17 @@
       <c r="F33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="2">
+        <v>9</v>
+      </c>
+      <c r="H33" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -2188,14 +2216,17 @@
       <c r="F34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="2">
+        <v>10</v>
+      </c>
+      <c r="H34" t="s">
         <v>59</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2208,14 +2239,17 @@
       <c r="E35" s="2">
         <v>2004</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="2">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
         <v>283</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -2231,14 +2265,17 @@
       <c r="F36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="2">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
         <v>108</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>124</v>
       </c>
@@ -2257,14 +2294,17 @@
       <c r="F37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="2">
+        <v>13</v>
+      </c>
+      <c r="H37" t="s">
         <v>102</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>124</v>
       </c>
@@ -2280,14 +2320,17 @@
       <c r="F38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="2">
+        <v>14</v>
+      </c>
+      <c r="H38" t="s">
         <v>81</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>124</v>
       </c>
@@ -2304,16 +2347,19 @@
         <v>2011</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="2">
+        <v>15</v>
+      </c>
+      <c r="H39" t="s">
         <v>104</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -2330,16 +2376,19 @@
         <v>2014</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="2">
+        <v>16</v>
+      </c>
+      <c r="H40" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -2356,16 +2405,19 @@
         <v>2017</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="2">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
         <v>106</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -2382,16 +2434,19 @@
         <v>2019</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="2">
+        <v>18</v>
+      </c>
+      <c r="H42" t="s">
         <v>98</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>124</v>
       </c>
@@ -2407,14 +2462,17 @@
       <c r="F43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="2">
+        <v>19</v>
+      </c>
+      <c r="H43" t="s">
         <v>94</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>124</v>
       </c>
@@ -2431,16 +2489,19 @@
         <v>2020</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="2">
+        <v>20</v>
+      </c>
+      <c r="H44" t="s">
         <v>112</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -2456,14 +2517,17 @@
       <c r="F45" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="2">
+        <v>21</v>
+      </c>
+      <c r="H45" t="s">
         <v>72</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>124</v>
       </c>
@@ -2479,14 +2543,17 @@
       <c r="F46" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="2">
+        <v>22</v>
+      </c>
+      <c r="H46" t="s">
         <v>121</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>124</v>
       </c>
@@ -2503,16 +2570,19 @@
         <v>2018</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G47" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="2">
+        <v>23</v>
+      </c>
+      <c r="H47" t="s">
         <v>119</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -2529,16 +2599,19 @@
         <v>2021</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G48" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="2">
+        <v>24</v>
+      </c>
+      <c r="H48" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>124</v>
       </c>
@@ -2554,14 +2627,17 @@
       <c r="F49" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="2">
+        <v>25</v>
+      </c>
+      <c r="H49" t="s">
         <v>86</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2578,16 +2654,19 @@
         <v>2010</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G50" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50" s="2">
+        <v>26</v>
+      </c>
+      <c r="H50" t="s">
         <v>90</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -2606,14 +2685,17 @@
       <c r="F51" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="2">
+        <v>27</v>
+      </c>
+      <c r="H51" t="s">
         <v>114</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -2629,14 +2711,17 @@
       <c r="F52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="2">
+        <v>28</v>
+      </c>
+      <c r="H52" t="s">
         <v>62</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>125</v>
       </c>
@@ -2652,14 +2737,17 @@
       <c r="F53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="2">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>156</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -2675,65 +2763,74 @@
       <c r="F54" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="2">
+        <v>2</v>
+      </c>
+      <c r="H54" t="s">
         <v>75</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>288</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E55">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G55" t="s">
-        <v>202</v>
+      <c r="G55" s="2">
+        <v>3</v>
       </c>
       <c r="H55" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="I55" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>216</v>
+        <v>288</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E56">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G56" t="s">
-        <v>200</v>
+        <v>50</v>
+      </c>
+      <c r="G56" s="2">
+        <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="I56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>216</v>
+        <v>288</v>
       </c>
       <c r="C57" t="s">
         <v>58</v>
@@ -2744,140 +2841,155 @@
       <c r="F57" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G57" t="s">
-        <v>206</v>
+      <c r="G57" s="2">
+        <v>5</v>
       </c>
       <c r="H57" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="I57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E58">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G58" t="s">
-        <v>210</v>
+      <c r="G58" s="2">
+        <v>6</v>
       </c>
       <c r="H58" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="I58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>216</v>
+        <v>289</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E59">
         <v>2020</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G59" t="s">
-        <v>208</v>
+        <v>50</v>
+      </c>
+      <c r="G59" s="2">
+        <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="I59" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>125</v>
       </c>
       <c r="B60" t="s">
-        <v>217</v>
+        <v>289</v>
       </c>
       <c r="C60" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E60">
-        <v>2016</v>
+        <v>1960</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G60" t="s">
-        <v>212</v>
+      <c r="G60" s="2">
+        <v>8</v>
       </c>
       <c r="H60" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="I60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>218</v>
+        <v>289</v>
       </c>
       <c r="C61" t="s">
         <v>58</v>
       </c>
       <c r="E61">
-        <v>2014</v>
+        <v>1998</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G61" t="s">
-        <v>214</v>
+      <c r="G61" s="2">
+        <v>9</v>
       </c>
       <c r="H61" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="I61" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>218</v>
+        <v>289</v>
       </c>
       <c r="C62" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E62">
-        <v>2021</v>
+        <v>2002</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G62" t="s">
-        <v>198</v>
+      <c r="G62" s="2">
+        <v>10</v>
       </c>
       <c r="H62" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="I62" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>290</v>
       </c>
       <c r="C63" t="s">
         <v>56</v>
@@ -2888,534 +3000,606 @@
       <c r="F63" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G63" t="s">
-        <v>196</v>
+      <c r="G63" s="2">
+        <v>11</v>
       </c>
       <c r="H63" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="I63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C64" t="s">
         <v>58</v>
       </c>
+      <c r="D64" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E64">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G64" t="s">
-        <v>150</v>
+      <c r="G64" s="2">
+        <v>12</v>
       </c>
       <c r="H64" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="I64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C65" t="s">
         <v>58</v>
       </c>
       <c r="E65">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G65" t="s">
-        <v>148</v>
+      <c r="G65" s="2">
+        <v>13</v>
       </c>
       <c r="H65" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="I65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C66" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E66">
-        <v>1974</v>
+        <v>2015</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G66" t="s">
-        <v>152</v>
+      <c r="G66" s="2">
+        <v>14</v>
       </c>
       <c r="H66" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="I66" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C67" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E67">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G67" t="s">
-        <v>154</v>
+      <c r="G67" s="2">
+        <v>15</v>
       </c>
       <c r="H67" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="I67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>289</v>
-      </c>
-      <c r="C68" t="s">
-        <v>58</v>
-      </c>
-      <c r="E68">
-        <v>1998</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G68" t="s">
-        <v>194</v>
+        <v>290</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" s="2">
+        <v>2018</v>
+      </c>
+      <c r="G68" s="2">
+        <v>16</v>
       </c>
       <c r="H68" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E69">
-        <v>2002</v>
+        <v>2021</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G69" t="s">
-        <v>190</v>
+      <c r="G69" s="2">
+        <v>17</v>
       </c>
       <c r="H69" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="I69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C70" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E70">
-        <v>1960</v>
+        <v>1998</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G70" t="s">
-        <v>146</v>
+      <c r="G70" s="2">
+        <v>18</v>
       </c>
       <c r="H70" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="I70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C71" t="s">
-        <v>56</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E71">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G71" t="s">
-        <v>192</v>
+      <c r="G71" s="2">
+        <v>19</v>
       </c>
       <c r="H71" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C72" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E72">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G72" t="s">
-        <v>184</v>
+        <v>50</v>
+      </c>
+      <c r="G72" s="2">
+        <v>20</v>
       </c>
       <c r="H72" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="I72" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E73">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G73" t="s">
-        <v>182</v>
+      <c r="G73" s="2">
+        <v>21</v>
       </c>
       <c r="H73" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="I73" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C74" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E74">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G74" t="s">
-        <v>188</v>
+      <c r="G74" s="2">
+        <v>22</v>
       </c>
       <c r="H74" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="I74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E75">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G75" t="s">
-        <v>180</v>
+      <c r="G75" s="2">
+        <v>23</v>
       </c>
       <c r="H75" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="I75" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>125</v>
       </c>
       <c r="B76" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C76" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E76">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G76" t="s">
-        <v>186</v>
+      <c r="G76" s="2">
+        <v>24</v>
       </c>
       <c r="H76" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="I76" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>125</v>
       </c>
       <c r="B77" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C77" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E77">
-        <v>1998</v>
+        <v>2018</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G77" t="s">
-        <v>158</v>
+      <c r="G77" s="2">
+        <v>25</v>
       </c>
       <c r="H77" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="I77" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>125</v>
       </c>
       <c r="B78" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C78" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E78">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G78" t="s">
-        <v>204</v>
+      <c r="G78" s="2">
+        <v>26</v>
       </c>
       <c r="H78" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="I78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>125</v>
       </c>
       <c r="B79" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C79" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E79">
-        <v>2021</v>
+        <v>1973</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G79" t="s">
-        <v>178</v>
+        <v>50</v>
+      </c>
+      <c r="G79" s="2">
+        <v>27</v>
       </c>
       <c r="H79" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="I79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>125</v>
       </c>
       <c r="B80" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C80" t="s">
         <v>56</v>
       </c>
       <c r="E80">
-        <v>2004</v>
+        <v>1988</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G80" t="s">
-        <v>174</v>
+      <c r="G80" s="2">
+        <v>28</v>
       </c>
       <c r="H80" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="I80" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>125</v>
       </c>
       <c r="B81" t="s">
-        <v>292</v>
+        <v>216</v>
       </c>
       <c r="C81" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E81">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G81" t="s">
-        <v>176</v>
+      <c r="G81" s="2">
+        <v>29</v>
       </c>
       <c r="H81" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="I81" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>125</v>
       </c>
       <c r="B82" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="C82" t="s">
         <v>58</v>
       </c>
       <c r="E82">
-        <v>2019</v>
+        <v>1975</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G82" t="s">
-        <v>168</v>
+        <v>50</v>
+      </c>
+      <c r="G82" s="2">
+        <v>30</v>
       </c>
       <c r="H82" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="I82" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>125</v>
       </c>
       <c r="B83" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="C83" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E83">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G83" t="s">
-        <v>170</v>
+        <v>50</v>
+      </c>
+      <c r="G83" s="2">
+        <v>31</v>
       </c>
       <c r="H83" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="I83" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>125</v>
       </c>
       <c r="B84" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="C84" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E84">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G84" t="s">
-        <v>172</v>
+      <c r="G84" s="2">
+        <v>32</v>
       </c>
       <c r="H84" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="I84" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>125</v>
       </c>
       <c r="B85" t="s">
-        <v>294</v>
+        <v>216</v>
       </c>
       <c r="C85" t="s">
         <v>58</v>
       </c>
       <c r="E85">
-        <v>1973</v>
+        <v>2020</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G85" t="s">
-        <v>166</v>
+      <c r="G85" s="2">
+        <v>33</v>
       </c>
       <c r="H85" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="I85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>294</v>
+        <v>217</v>
       </c>
       <c r="C86" t="s">
         <v>56</v>
@@ -3424,68 +3608,74 @@
         <v>50</v>
       </c>
       <c r="E86">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G86" t="s">
-        <v>164</v>
+      <c r="G86" s="2">
+        <v>34</v>
       </c>
       <c r="H86" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="I86" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="C87" t="s">
         <v>56</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E87">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G87" t="s">
-        <v>160</v>
+      <c r="G87" s="2">
+        <v>35</v>
       </c>
       <c r="H87" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="I87" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>125</v>
       </c>
       <c r="B88" t="s">
-        <v>295</v>
+        <v>218</v>
       </c>
       <c r="C88" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E88">
-        <v>1988</v>
+        <v>2014</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G88" t="s">
-        <v>162</v>
+      <c r="G88" s="2">
+        <v>36</v>
       </c>
       <c r="H88" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I88" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>220</v>
       </c>
@@ -3501,14 +3691,17 @@
       <c r="E89">
         <v>2019</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="2">
+        <v>1</v>
+      </c>
+      <c r="H89" t="s">
         <v>249</v>
       </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>220</v>
       </c>
@@ -3524,14 +3717,17 @@
       <c r="E90">
         <v>2020</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="2">
+        <v>2</v>
+      </c>
+      <c r="H90" t="s">
         <v>265</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>220</v>
       </c>
@@ -3547,14 +3743,20 @@
       <c r="E91">
         <v>2003</v>
       </c>
-      <c r="G91" t="s">
+      <c r="F91" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G91" s="2">
+        <v>3</v>
+      </c>
+      <c r="H91" t="s">
         <v>263</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>220</v>
       </c>
@@ -3570,14 +3772,20 @@
       <c r="E92">
         <v>2013</v>
       </c>
-      <c r="G92" t="s">
+      <c r="F92" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G92" s="2">
+        <v>4</v>
+      </c>
+      <c r="H92" t="s">
         <v>261</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>220</v>
       </c>
@@ -3593,14 +3801,17 @@
       <c r="E93">
         <v>2019</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="2">
+        <v>5</v>
+      </c>
+      <c r="H93" t="s">
         <v>34</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>220</v>
       </c>
@@ -3613,14 +3824,17 @@
       <c r="E94">
         <v>2019</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="2">
+        <v>6</v>
+      </c>
+      <c r="H94" t="s">
         <v>243</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>220</v>
       </c>
@@ -3636,14 +3850,17 @@
       <c r="E95">
         <v>2015</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" s="2">
+        <v>7</v>
+      </c>
+      <c r="H95" t="s">
         <v>259</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -3656,14 +3873,17 @@
       <c r="E96">
         <v>2016</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="2">
+        <v>8</v>
+      </c>
+      <c r="H96" t="s">
         <v>257</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>220</v>
       </c>
@@ -3676,14 +3896,17 @@
       <c r="E97">
         <v>1972</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" s="2">
+        <v>9</v>
+      </c>
+      <c r="H97" t="s">
         <v>92</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>220</v>
       </c>
@@ -3699,14 +3922,17 @@
       <c r="E98">
         <v>2007</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="2">
+        <v>10</v>
+      </c>
+      <c r="H98" t="s">
         <v>255</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>220</v>
       </c>
@@ -3719,14 +3945,17 @@
       <c r="E99">
         <v>2013</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="2">
+        <v>11</v>
+      </c>
+      <c r="H99" t="s">
         <v>253</v>
       </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>220</v>
       </c>
@@ -3742,14 +3971,20 @@
       <c r="E100">
         <v>2016</v>
       </c>
-      <c r="G100" t="s">
+      <c r="F100" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G100" s="2">
+        <v>12</v>
+      </c>
+      <c r="H100" t="s">
         <v>65</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>220</v>
       </c>
@@ -3762,14 +3997,17 @@
       <c r="E101">
         <v>2018</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G101" s="2">
+        <v>13</v>
+      </c>
+      <c r="H101" t="s">
         <v>241</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>220</v>
       </c>
@@ -3782,14 +4020,17 @@
       <c r="E102">
         <v>2020</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" s="2">
+        <v>14</v>
+      </c>
+      <c r="H102" t="s">
         <v>41</v>
       </c>
-      <c r="H102" t="s">
+      <c r="I102" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>220</v>
       </c>
@@ -3802,14 +4043,17 @@
       <c r="E103">
         <v>1999</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G103" s="2">
+        <v>15</v>
+      </c>
+      <c r="H103" t="s">
         <v>69</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>220</v>
       </c>
@@ -3822,14 +4066,17 @@
       <c r="E104">
         <v>2005</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G104" s="2">
+        <v>16</v>
+      </c>
+      <c r="H104" t="s">
         <v>245</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>220</v>
       </c>
@@ -3845,14 +4092,17 @@
       <c r="E105">
         <v>2008</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G105" s="2">
+        <v>17</v>
+      </c>
+      <c r="H105" t="s">
         <v>247</v>
       </c>
-      <c r="H105" t="s">
+      <c r="I105" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>220</v>
       </c>
@@ -3865,14 +4115,17 @@
       <c r="E106">
         <v>2019</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G106" s="2">
+        <v>18</v>
+      </c>
+      <c r="H106" t="s">
         <v>98</v>
       </c>
-      <c r="H106" t="s">
+      <c r="I106" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>220</v>
       </c>
@@ -3885,14 +4138,17 @@
       <c r="E107">
         <v>2007</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" s="2">
+        <v>19</v>
+      </c>
+      <c r="H107" t="s">
         <v>67</v>
       </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -3905,14 +4161,17 @@
       <c r="E108">
         <v>2013</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G108" s="2">
+        <v>20</v>
+      </c>
+      <c r="H108" t="s">
         <v>21</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -3925,14 +4184,17 @@
       <c r="E109">
         <v>1989</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G109" s="2">
+        <v>21</v>
+      </c>
+      <c r="H109" t="s">
         <v>239</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>220</v>
       </c>
@@ -3948,14 +4210,17 @@
       <c r="E110">
         <v>2012</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G110" s="2">
+        <v>22</v>
+      </c>
+      <c r="H110" t="s">
         <v>267</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>220</v>
       </c>
@@ -3971,14 +4236,17 @@
       <c r="E111">
         <v>2012</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111" s="2">
+        <v>23</v>
+      </c>
+      <c r="H111" t="s">
         <v>251</v>
       </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>220</v>
       </c>
@@ -3994,14 +4262,17 @@
       <c r="E112">
         <v>2013</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G112" s="2">
+        <v>24</v>
+      </c>
+      <c r="H112" t="s">
         <v>237</v>
       </c>
-      <c r="H112" t="s">
+      <c r="I112" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>220</v>
       </c>
@@ -4017,14 +4288,17 @@
       <c r="E113">
         <v>2015</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G113" s="2">
+        <v>25</v>
+      </c>
+      <c r="H113" t="s">
         <v>3</v>
       </c>
-      <c r="H113" t="s">
+      <c r="I113" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>220</v>
       </c>
@@ -4040,14 +4314,17 @@
       <c r="E114">
         <v>2020</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114" s="2">
+        <v>26</v>
+      </c>
+      <c r="H114" t="s">
         <v>119</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>220</v>
       </c>
@@ -4063,14 +4340,17 @@
       <c r="E115">
         <v>2022</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G115" s="2">
+        <v>27</v>
+      </c>
+      <c r="H115" t="s">
         <v>3</v>
       </c>
-      <c r="H115" t="s">
+      <c r="I115" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>220</v>
       </c>
@@ -4083,14 +4363,17 @@
       <c r="E116">
         <v>2015</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G116" s="2">
+        <v>28</v>
+      </c>
+      <c r="H116" t="s">
         <v>233</v>
       </c>
-      <c r="H116" t="s">
+      <c r="I116" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>220</v>
       </c>
@@ -4106,14 +4389,17 @@
       <c r="E117">
         <v>2015</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G117" s="2">
+        <v>29</v>
+      </c>
+      <c r="H117" t="s">
         <v>231</v>
       </c>
-      <c r="H117" t="s">
+      <c r="I117" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>220</v>
       </c>
@@ -4129,14 +4415,17 @@
       <c r="E118">
         <v>2020</v>
       </c>
-      <c r="G118" t="s">
+      <c r="G118" s="2">
+        <v>30</v>
+      </c>
+      <c r="H118" t="s">
         <v>229</v>
       </c>
-      <c r="H118" t="s">
+      <c r="I118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>220</v>
       </c>
@@ -4149,14 +4438,17 @@
       <c r="E119">
         <v>2018</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G119" s="2">
+        <v>31</v>
+      </c>
+      <c r="H119" t="s">
         <v>221</v>
       </c>
-      <c r="H119" t="s">
+      <c r="I119" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>220</v>
       </c>
@@ -4172,14 +4464,17 @@
       <c r="E120">
         <v>2021</v>
       </c>
-      <c r="G120" t="s">
+      <c r="G120" s="2">
+        <v>32</v>
+      </c>
+      <c r="H120" t="s">
         <v>223</v>
       </c>
-      <c r="H120" t="s">
+      <c r="I120" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>220</v>
       </c>
@@ -4195,14 +4490,17 @@
       <c r="E121">
         <v>2022</v>
       </c>
-      <c r="G121" t="s">
+      <c r="G121" s="2">
+        <v>33</v>
+      </c>
+      <c r="H121" t="s">
         <v>225</v>
       </c>
-      <c r="H121" t="s">
+      <c r="I121" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>220</v>
       </c>
@@ -4218,14 +4516,17 @@
       <c r="E122">
         <v>2022</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122" s="2">
+        <v>34</v>
+      </c>
+      <c r="H122" t="s">
         <v>227</v>
       </c>
-      <c r="H122" t="s">
+      <c r="I122" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -4241,34 +4542,43 @@
       <c r="F123" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" s="2">
+        <v>29</v>
+      </c>
+      <c r="H123" t="s">
         <v>96</v>
       </c>
-      <c r="H123" s="1" t="s">
+      <c r="I123" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>290</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E124" s="2">
-        <v>2018</v>
-      </c>
-      <c r="G124" t="s">
-        <v>286</v>
-      </c>
-      <c r="H124" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="C124" t="s">
+        <v>56</v>
+      </c>
+      <c r="E124">
+        <v>2015</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G124" s="2">
+        <v>37</v>
+      </c>
+      <c r="H124" t="s">
+        <v>196</v>
+      </c>
+      <c r="I124" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>220</v>
       </c>
@@ -4284,11 +4594,14 @@
       <c r="E125" s="2">
         <v>1994</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G125" s="2">
+        <v>35</v>
+      </c>
+      <c r="H125" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>220</v>
       </c>
@@ -4301,22 +4614,25 @@
       <c r="E126" s="2">
         <v>2010</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126" s="2">
+        <v>36</v>
+      </c>
+      <c r="H126" t="s">
         <v>1</v>
       </c>
-      <c r="H126" s="1" t="s">
+      <c r="I126" s="1" t="s">
         <v>297</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H126" xr:uid="{2AC9AABE-D912-4539-92BB-AE21E65F9BAF}">
+  <autoFilter ref="A1:I126" xr:uid="{2AC9AABE-D912-4539-92BB-AE21E65F9BAF}">
     <filterColumn colId="0">
       <filters>
-        <filter val="2 Shapiro"/>
+        <filter val="4 Walker"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:H123">
-      <sortCondition ref="A1:A126"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:I124">
+      <sortCondition ref="B1:B126"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>